<commit_message>
Adding stuff to git, init!!
</commit_message>
<xml_diff>
--- a/ShoeSizes.xlsx
+++ b/ShoeSizes.xlsx
@@ -12,9 +12,13 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -120,6 +124,15 @@
   </si>
   <si>
     <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Average of Shoe Size</t>
   </si>
 </sst>
 </file>
@@ -155,8 +168,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,6 +190,281 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43052.615545949076" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="14">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D15" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Eye color" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Brown"/>
+        <s v="Green"/>
+        <s v="Blue"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Location" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Birmingham"/>
+        <s v="Brussels"/>
+        <s v="Dusseldoorf"/>
+        <s v="Edinburgh"/>
+        <s v="Hampstead"/>
+        <s v="Leven"/>
+        <s v="Manchester"/>
+        <s v="Solihull"/>
+        <s v="Torquay"/>
+        <s v="Whitby"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Shoe Size" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="14" count="8">
+        <n v="10"/>
+        <n v="6"/>
+        <n v="8"/>
+        <n v="7"/>
+        <n v="12"/>
+        <n v="4"/>
+        <n v="13"/>
+        <n v="14"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="14">
+  <r>
+    <s v="Wilson"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Lawrence"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Philip"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="Tom"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Susan"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="Joan"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Fiona"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Alastair"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="Sally"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="John"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Vicky"/>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="Ryan"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="David"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="Wendy"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="9">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="24">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Shoe Size" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,10 +730,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="222" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="3">
+        <v>9.1428571428571423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="207" workbookViewId="0">
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,30 +973,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -514,30 +1029,30 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,27 +1071,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -584,13 +1099,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -598,30 +1113,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -640,19 +1155,22 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D15">
+    <sortCondition ref="C2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>